<commit_message>
Cleanup. Statistics about image compression.
</commit_message>
<xml_diff>
--- a/assets/savedSpaceByImageCompression.xlsx
+++ b/assets/savedSpaceByImageCompression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Elephant/Users/uwe/Documents/BC-projects/Development/html/EO4SD Dissemination Platform/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F1C1B8-5CE4-2443-8029-D4E12FF0152B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D84369-DCC2-4742-82F3-4F6F03D438E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5500" windowWidth="28040" windowHeight="21460" xr2:uid="{719E5152-29F4-104E-98F5-853B818EE6D2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>before</t>
   </si>
@@ -193,6 +193,78 @@
   </si>
   <si>
     <t>.../WesternIndianOcean_chla_20200604_ql.png</t>
+  </si>
+  <si>
+    <t>data/Caribbean/Caribbean_chla_20200412.png</t>
+  </si>
+  <si>
+    <t>data/Caribbean/Caribbean_chla_20200412_ql.png</t>
+  </si>
+  <si>
+    <t>data/Caribbean/dominica_shoreline_2019.PNG</t>
+  </si>
+  <si>
+    <t>data/Caribbean/dominica_shoreline_2019.jpg</t>
+  </si>
+  <si>
+    <t>data/Caribbean/grenada_shoreline_2019.PNG</t>
+  </si>
+  <si>
+    <t>data/Caribbean/grenada_shoreline_2019.jpg</t>
+  </si>
+  <si>
+    <t>data/Caribbean/stkitts_shoreline_2019.PNG</t>
+  </si>
+  <si>
+    <t>data/Caribbean/stkitts_shoreline_2019.jpg</t>
+  </si>
+  <si>
+    <t>data/Caribbean/stlucia_shoreline_2019.PNG</t>
+  </si>
+  <si>
+    <t>data/Caribbean/stlucia_shoreline_2019.jpg</t>
+  </si>
+  <si>
+    <t>data/Caribbean/stvincent_shoreline_2019.jpg</t>
+  </si>
+  <si>
+    <t>data/Caribbean/stvincent_shoreline_2019.png</t>
+  </si>
+  <si>
+    <t>data/Caribbean/wq/caribbean_chl.png</t>
+  </si>
+  <si>
+    <t>data/Caribbean/wq/caribbean_chl_quicklook.png</t>
+  </si>
+  <si>
+    <t>data/Caribbean/wq/caribbean_tsm.png</t>
+  </si>
+  <si>
+    <t>data/Caribbean/wq/caribbean_tsm_quicklook.png</t>
+  </si>
+  <si>
+    <t>data/NorthAfrica/NorthAfrica_chla_20200524.png</t>
+  </si>
+  <si>
+    <t>data/NorthAfrica/NorthAfrica_chla_20200524_ql.png</t>
+  </si>
+  <si>
+    <t>data/NorthAfrica/Tunisia/Tunisia_quicklook.jpg</t>
+  </si>
+  <si>
+    <t>data/SoutheastAsia/Philippines/eo4sd_philippines_v1_finfish_mean_stock_density.png</t>
+  </si>
+  <si>
+    <t>data/SoutheastAsia/Philippines/eo4sd_philippines_v1_finfish_mean_stock_density_ql.png</t>
+  </si>
+  <si>
+    <t>data/SoutheastAsia/Philippines/eo4sd_philippines_v1_finfish_site_selection.png</t>
+  </si>
+  <si>
+    <t>data/SoutheastAsia/Philippines/eo4sd_philippines_v1_finfish_site_selection_ql.png</t>
+  </si>
+  <si>
+    <t>images/dummy.png</t>
   </si>
 </sst>
 </file>
@@ -239,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -250,6 +322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -564,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D806A48-ED72-0849-8E9A-12CEF63F99B8}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -785,13 +858,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="B12">
-        <v>3883376</v>
+        <v>201822</v>
       </c>
       <c r="C12">
-        <v>510382</v>
+        <v>25831</v>
       </c>
       <c r="D12" s="5" t="str">
         <f>RIGHT(A12,3)</f>
@@ -799,18 +872,18 @@
       </c>
       <c r="E12" s="1">
         <f>C12/B12</f>
-        <v>0.13142739719254587</v>
+        <v>0.12798902002754903</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B13">
-        <v>6014206</v>
+        <v>141078</v>
       </c>
       <c r="C13">
-        <v>866156</v>
+        <v>18511</v>
       </c>
       <c r="D13" s="5" t="str">
         <f>RIGHT(A13,3)</f>
@@ -818,18 +891,18 @@
       </c>
       <c r="E13" s="1">
         <f>C13/B13</f>
-        <v>0.14401834589636603</v>
+        <v>0.13121110307773004</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B14">
-        <v>270341</v>
+        <v>3883376</v>
       </c>
       <c r="C14">
-        <v>40632</v>
+        <v>510382</v>
       </c>
       <c r="D14" s="5" t="str">
         <f>RIGHT(A14,3)</f>
@@ -837,18 +910,18 @@
       </c>
       <c r="E14" s="1">
         <f>C14/B14</f>
-        <v>0.15029906673423565</v>
+        <v>0.13142739719254587</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B15">
-        <v>5472452</v>
+        <v>170997</v>
       </c>
       <c r="C15">
-        <v>830966</v>
+        <v>22543</v>
       </c>
       <c r="D15" s="5" t="str">
         <f>RIGHT(A15,3)</f>
@@ -856,18 +929,18 @@
       </c>
       <c r="E15" s="1">
         <f>C15/B15</f>
-        <v>0.15184527886219926</v>
+        <v>0.13183272221150077</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B16">
-        <v>3824920</v>
+        <v>156551</v>
       </c>
       <c r="C16">
-        <v>592220</v>
+        <v>20743</v>
       </c>
       <c r="D16" s="5" t="str">
         <f>RIGHT(A16,3)</f>
@@ -875,18 +948,18 @@
       </c>
       <c r="E16" s="1">
         <f>C16/B16</f>
-        <v>0.15483199648620102</v>
+        <v>0.1324999520922894</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17">
-        <v>161202</v>
+        <v>6014206</v>
       </c>
       <c r="C17">
-        <v>25263</v>
+        <v>866156</v>
       </c>
       <c r="D17" s="5" t="str">
         <f>RIGHT(A17,3)</f>
@@ -894,37 +967,37 @@
       </c>
       <c r="E17" s="1">
         <f>C17/B17</f>
-        <v>0.15671641791044777</v>
+        <v>0.14401834589636603</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="B18">
-        <v>216625</v>
+        <v>118069</v>
       </c>
       <c r="C18">
-        <v>40653</v>
+        <v>17465</v>
       </c>
       <c r="D18" s="5" t="str">
         <f>RIGHT(A18,3)</f>
-        <v>JPG</v>
+        <v>jpg</v>
       </c>
       <c r="E18" s="1">
         <f>C18/B18</f>
-        <v>0.18766532025389498</v>
+        <v>0.14792197782652516</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B19">
-        <v>180997</v>
+        <v>270341</v>
       </c>
       <c r="C19">
-        <v>36774</v>
+        <v>40632</v>
       </c>
       <c r="D19" s="5" t="str">
         <f>RIGHT(A19,3)</f>
@@ -932,18 +1005,18 @@
       </c>
       <c r="E19" s="1">
         <f>C19/B19</f>
-        <v>0.20317463825367271</v>
+        <v>0.15029906673423565</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B20">
-        <v>315663</v>
+        <v>5472452</v>
       </c>
       <c r="C20">
-        <v>65625</v>
+        <v>830966</v>
       </c>
       <c r="D20" s="5" t="str">
         <f>RIGHT(A20,3)</f>
@@ -951,18 +1024,18 @@
       </c>
       <c r="E20" s="1">
         <f>C20/B20</f>
-        <v>0.20789576225278225</v>
+        <v>0.15184527886219926</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>232566</v>
+        <v>3824920</v>
       </c>
       <c r="C21">
-        <v>49686</v>
+        <v>592220</v>
       </c>
       <c r="D21" s="5" t="str">
         <f>RIGHT(A21,3)</f>
@@ -970,132 +1043,132 @@
       </c>
       <c r="E21" s="1">
         <f>C21/B21</f>
-        <v>0.21364257888083382</v>
+        <v>0.15483199648620102</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B22">
-        <v>1303470</v>
+        <v>161202</v>
       </c>
       <c r="C22">
-        <v>382283</v>
+        <v>25263</v>
       </c>
       <c r="D22" s="5" t="str">
         <f>RIGHT(A22,3)</f>
-        <v>png</v>
+        <v>jpg</v>
       </c>
       <c r="E22" s="1">
         <f>C22/B22</f>
-        <v>0.2932810114540419</v>
+        <v>0.15671641791044777</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B23">
-        <v>108835</v>
+        <v>216625</v>
       </c>
       <c r="C23">
-        <v>32568</v>
+        <v>40653</v>
       </c>
       <c r="D23" s="5" t="str">
         <f>RIGHT(A23,3)</f>
-        <v>png</v>
+        <v>JPG</v>
       </c>
       <c r="E23" s="1">
         <f>C23/B23</f>
-        <v>0.29924197179216244</v>
+        <v>0.18766532025389498</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>31131</v>
+        <v>180997</v>
       </c>
       <c r="C24">
-        <v>9638</v>
+        <v>36774</v>
       </c>
       <c r="D24" s="5" t="str">
         <f>RIGHT(A24,3)</f>
-        <v>png</v>
+        <v>jpg</v>
       </c>
       <c r="E24" s="1">
         <f>C24/B24</f>
-        <v>0.30959493752208411</v>
+        <v>0.20317463825367271</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B25">
-        <v>129963</v>
+        <v>315663</v>
       </c>
       <c r="C25">
-        <v>44568</v>
+        <v>65625</v>
       </c>
       <c r="D25" s="5" t="str">
         <f>RIGHT(A25,3)</f>
-        <v>png</v>
+        <v>jpg</v>
       </c>
       <c r="E25" s="1">
         <f>C25/B25</f>
-        <v>0.34292837192123909</v>
+        <v>0.20789576225278225</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B26">
-        <v>38323</v>
+        <v>232566</v>
       </c>
       <c r="C26">
-        <v>13404</v>
+        <v>49686</v>
       </c>
       <c r="D26" s="5" t="str">
         <f>RIGHT(A26,3)</f>
-        <v>png</v>
+        <v>jpg</v>
       </c>
       <c r="E26" s="1">
         <f>C26/B26</f>
-        <v>0.34976384938548655</v>
+        <v>0.21364257888083382</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="B27">
-        <v>71958</v>
+        <v>249044</v>
       </c>
       <c r="C27">
-        <v>25463</v>
+        <v>55418</v>
       </c>
       <c r="D27" s="5" t="str">
         <f>RIGHT(A27,3)</f>
-        <v>png</v>
+        <v>jpg</v>
       </c>
       <c r="E27" s="1">
         <f>C27/B27</f>
-        <v>0.35385919564190221</v>
+        <v>0.22252292767543086</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B28">
-        <v>104911</v>
+        <v>1303470</v>
       </c>
       <c r="C28">
-        <v>37368</v>
+        <v>382283</v>
       </c>
       <c r="D28" s="5" t="str">
         <f>RIGHT(A28,3)</f>
@@ -1103,18 +1176,18 @@
       </c>
       <c r="E28" s="1">
         <f>C28/B28</f>
-        <v>0.3561876257017853</v>
+        <v>0.2932810114540419</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B29">
-        <v>592813</v>
+        <v>108835</v>
       </c>
       <c r="C29">
-        <v>214113</v>
+        <v>32568</v>
       </c>
       <c r="D29" s="5" t="str">
         <f>RIGHT(A29,3)</f>
@@ -1122,75 +1195,75 @@
       </c>
       <c r="E29" s="1">
         <f>C29/B29</f>
-        <v>0.36118135061140699</v>
+        <v>0.29924197179216244</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B30">
-        <v>99320</v>
+        <v>48327</v>
       </c>
       <c r="C30">
-        <v>36047</v>
+        <v>14517</v>
       </c>
       <c r="D30" s="5" t="str">
         <f>RIGHT(A30,3)</f>
-        <v>png</v>
+        <v>PNG</v>
       </c>
       <c r="E30" s="1">
         <f>C30/B30</f>
-        <v>0.36293797825211438</v>
+        <v>0.30039108572847478</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B31">
-        <v>732692</v>
+        <v>42125</v>
       </c>
       <c r="C31">
-        <v>270414</v>
+        <v>12974</v>
       </c>
       <c r="D31" s="5" t="str">
         <f>RIGHT(A31,3)</f>
-        <v>png</v>
+        <v>PNG</v>
       </c>
       <c r="E31" s="1">
         <f>C31/B31</f>
-        <v>0.36906913136761421</v>
+        <v>0.3079881305637982</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B32">
-        <v>596140</v>
+        <v>53662</v>
       </c>
       <c r="C32">
-        <v>220604</v>
+        <v>16549</v>
       </c>
       <c r="D32" s="5" t="str">
         <f>RIGHT(A32,3)</f>
-        <v>png</v>
+        <v>PNG</v>
       </c>
       <c r="E32" s="1">
         <f>C32/B32</f>
-        <v>0.37005401415774819</v>
+        <v>0.30839327643397563</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B33">
-        <v>794917</v>
+        <v>31131</v>
       </c>
       <c r="C33">
-        <v>300100</v>
+        <v>9638</v>
       </c>
       <c r="D33" s="5" t="str">
         <f>RIGHT(A33,3)</f>
@@ -1198,37 +1271,37 @@
       </c>
       <c r="E33" s="1">
         <f>C33/B33</f>
-        <v>0.37752369115266121</v>
+        <v>0.30959493752208411</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B34">
-        <v>103718</v>
+        <v>53851</v>
       </c>
       <c r="C34">
-        <v>39559</v>
+        <v>16739</v>
       </c>
       <c r="D34" s="5" t="str">
         <f>RIGHT(A34,3)</f>
-        <v>png</v>
+        <v>PNG</v>
       </c>
       <c r="E34" s="1">
         <f>C34/B34</f>
-        <v>0.38140920573092424</v>
+        <v>0.31083916733208294</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B35">
-        <v>607591</v>
+        <v>45078</v>
       </c>
       <c r="C35">
-        <v>232884</v>
+        <v>14098</v>
       </c>
       <c r="D35" s="5" t="str">
         <f>RIGHT(A35,3)</f>
@@ -1236,18 +1309,18 @@
       </c>
       <c r="E35" s="1">
         <f>C35/B35</f>
-        <v>0.3832907334045435</v>
+        <v>0.31274679444518388</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="B36">
-        <v>362496</v>
+        <v>251396</v>
       </c>
       <c r="C36">
-        <v>140096</v>
+        <v>81297</v>
       </c>
       <c r="D36" s="5" t="str">
         <f>RIGHT(A36,3)</f>
@@ -1255,18 +1328,18 @@
       </c>
       <c r="E36" s="1">
         <f>C36/B36</f>
-        <v>0.38647598870056499</v>
+        <v>0.32338223360753554</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="B37">
-        <v>182490</v>
+        <v>46405</v>
       </c>
       <c r="C37">
-        <v>71410</v>
+        <v>15561</v>
       </c>
       <c r="D37" s="5" t="str">
         <f>RIGHT(A37,3)</f>
@@ -1274,18 +1347,18 @@
       </c>
       <c r="E37" s="1">
         <f>C37/B37</f>
-        <v>0.39130911282810016</v>
+        <v>0.33533024458571276</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B38">
-        <v>284286</v>
+        <v>43435</v>
       </c>
       <c r="C38">
-        <v>113724</v>
+        <v>14669</v>
       </c>
       <c r="D38" s="5" t="str">
         <f>RIGHT(A38,3)</f>
@@ -1293,18 +1366,18 @@
       </c>
       <c r="E38" s="1">
         <f>C38/B38</f>
-        <v>0.40003376881028258</v>
+        <v>0.33772303441924717</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B39">
-        <v>116510</v>
+        <v>129963</v>
       </c>
       <c r="C39">
-        <v>46835</v>
+        <v>44568</v>
       </c>
       <c r="D39" s="5" t="str">
         <f>RIGHT(A39,3)</f>
@@ -1312,18 +1385,18 @@
       </c>
       <c r="E39" s="1">
         <f>C39/B39</f>
-        <v>0.40198266243240921</v>
+        <v>0.34292837192123909</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="B40">
-        <v>197231</v>
+        <v>27647</v>
       </c>
       <c r="C40">
-        <v>79783</v>
+        <v>9649</v>
       </c>
       <c r="D40" s="5" t="str">
         <f>RIGHT(A40,3)</f>
@@ -1331,18 +1404,18 @@
       </c>
       <c r="E40" s="1">
         <f>C40/B40</f>
-        <v>0.40451551733753821</v>
+        <v>0.34900712554707564</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B41">
-        <v>20915</v>
+        <v>38323</v>
       </c>
       <c r="C41">
-        <v>8561</v>
+        <v>13404</v>
       </c>
       <c r="D41" s="5" t="str">
         <f>RIGHT(A41,3)</f>
@@ -1350,18 +1423,18 @@
       </c>
       <c r="E41" s="1">
         <f>C41/B41</f>
-        <v>0.40932345206789383</v>
+        <v>0.34976384938548655</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B42">
-        <v>453740</v>
+        <v>71958</v>
       </c>
       <c r="C42">
-        <v>194150</v>
+        <v>25463</v>
       </c>
       <c r="D42" s="5" t="str">
         <f>RIGHT(A42,3)</f>
@@ -1369,18 +1442,18 @@
       </c>
       <c r="E42" s="1">
         <f>C42/B42</f>
-        <v>0.42788821792215809</v>
+        <v>0.35385919564190221</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B43">
-        <v>143856</v>
+        <v>104911</v>
       </c>
       <c r="C43">
-        <v>62041</v>
+        <v>37368</v>
       </c>
       <c r="D43" s="5" t="str">
         <f>RIGHT(A43,3)</f>
@@ -1388,18 +1461,18 @@
       </c>
       <c r="E43" s="1">
         <f>C43/B43</f>
-        <v>0.43127154932710488</v>
+        <v>0.3561876257017853</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B44">
-        <v>1164813</v>
+        <v>592813</v>
       </c>
       <c r="C44">
-        <v>534807</v>
+        <v>214113</v>
       </c>
       <c r="D44" s="5" t="str">
         <f>RIGHT(A44,3)</f>
@@ -1407,18 +1480,18 @@
       </c>
       <c r="E44" s="1">
         <f>C44/B44</f>
-        <v>0.45913550071985804</v>
+        <v>0.36118135061140699</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B45">
-        <v>146028</v>
+        <v>99320</v>
       </c>
       <c r="C45">
-        <v>67593</v>
+        <v>36047</v>
       </c>
       <c r="D45" s="5" t="str">
         <f>RIGHT(A45,3)</f>
@@ -1426,18 +1499,18 @@
       </c>
       <c r="E45" s="1">
         <f>C45/B45</f>
-        <v>0.46287698249650749</v>
+        <v>0.36293797825211438</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B46">
-        <v>4222419</v>
+        <v>732692</v>
       </c>
       <c r="C46">
-        <v>2018199</v>
+        <v>270414</v>
       </c>
       <c r="D46" s="5" t="str">
         <f>RIGHT(A46,3)</f>
@@ -1445,18 +1518,18 @@
       </c>
       <c r="E46" s="1">
         <f>C46/B46</f>
-        <v>0.4779722239787193</v>
+        <v>0.36906913136761421</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B47">
-        <v>433723</v>
+        <v>596140</v>
       </c>
       <c r="C47">
-        <v>211545</v>
+        <v>220604</v>
       </c>
       <c r="D47" s="5" t="str">
         <f>RIGHT(A47,3)</f>
@@ -1464,18 +1537,18 @@
       </c>
       <c r="E47" s="1">
         <f>C47/B47</f>
-        <v>0.48774217645824641</v>
+        <v>0.37005401415774819</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="B48">
-        <v>471610</v>
+        <v>38892</v>
       </c>
       <c r="C48">
-        <v>238069</v>
+        <v>14531</v>
       </c>
       <c r="D48" s="5" t="str">
         <f>RIGHT(A48,3)</f>
@@ -1483,18 +1556,18 @@
       </c>
       <c r="E48" s="1">
         <f>C48/B48</f>
-        <v>0.50480057674773648</v>
+        <v>0.37362439576262468</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B49">
-        <v>361228</v>
+        <v>37592</v>
       </c>
       <c r="C49">
-        <v>220292</v>
+        <v>14080</v>
       </c>
       <c r="D49" s="5" t="str">
         <f>RIGHT(A49,3)</f>
@@ -1502,28 +1575,484 @@
       </c>
       <c r="E49" s="1">
         <f>C49/B49</f>
+        <v>0.37454777612257928</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50">
+        <v>794917</v>
+      </c>
+      <c r="C50">
+        <v>300100</v>
+      </c>
+      <c r="D50" s="5" t="str">
+        <f>RIGHT(A50,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E50" s="1">
+        <f>C50/B50</f>
+        <v>0.37752369115266121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51">
+        <v>103718</v>
+      </c>
+      <c r="C51">
+        <v>39559</v>
+      </c>
+      <c r="D51" s="5" t="str">
+        <f>RIGHT(A51,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E51" s="1">
+        <f>C51/B51</f>
+        <v>0.38140920573092424</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52">
+        <v>607591</v>
+      </c>
+      <c r="C52">
+        <v>232884</v>
+      </c>
+      <c r="D52" s="5" t="str">
+        <f>RIGHT(A52,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E52" s="1">
+        <f>C52/B52</f>
+        <v>0.3832907334045435</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53">
+        <v>49352</v>
+      </c>
+      <c r="C53">
+        <v>19054</v>
+      </c>
+      <c r="D53" s="5" t="str">
+        <f>RIGHT(A53,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E53" s="1">
+        <f>C53/B53</f>
+        <v>0.38608364402658452</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54">
+        <v>362496</v>
+      </c>
+      <c r="C54">
+        <v>140096</v>
+      </c>
+      <c r="D54" s="5" t="str">
+        <f>RIGHT(A54,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E54" s="1">
+        <f>C54/B54</f>
+        <v>0.38647598870056499</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55">
+        <v>299628</v>
+      </c>
+      <c r="C55">
+        <v>117140</v>
+      </c>
+      <c r="D55" s="5" t="str">
+        <f>RIGHT(A55,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E55" s="1">
+        <f>C55/B55</f>
+        <v>0.39095144646027741</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56">
+        <v>182490</v>
+      </c>
+      <c r="C56">
+        <v>71410</v>
+      </c>
+      <c r="D56" s="5" t="str">
+        <f>RIGHT(A56,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E56" s="1">
+        <f>C56/B56</f>
+        <v>0.39130911282810016</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57">
+        <v>1172756</v>
+      </c>
+      <c r="C57">
+        <v>466441</v>
+      </c>
+      <c r="D57" s="5" t="str">
+        <f>RIGHT(A57,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E57" s="1">
+        <f>C57/B57</f>
+        <v>0.39773064473769482</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58">
+        <v>284286</v>
+      </c>
+      <c r="C58">
+        <v>113724</v>
+      </c>
+      <c r="D58" s="5" t="str">
+        <f>RIGHT(A58,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E58" s="1">
+        <f>C58/B58</f>
+        <v>0.40003376881028258</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59">
+        <v>116510</v>
+      </c>
+      <c r="C59">
+        <v>46835</v>
+      </c>
+      <c r="D59" s="5" t="str">
+        <f>RIGHT(A59,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E59" s="1">
+        <f>C59/B59</f>
+        <v>0.40198266243240921</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60">
+        <v>197231</v>
+      </c>
+      <c r="C60">
+        <v>79783</v>
+      </c>
+      <c r="D60" s="5" t="str">
+        <f>RIGHT(A60,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E60" s="1">
+        <f>C60/B60</f>
+        <v>0.40451551733753821</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61">
+        <v>20915</v>
+      </c>
+      <c r="C61">
+        <v>8561</v>
+      </c>
+      <c r="D61" s="5" t="str">
+        <f>RIGHT(A61,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E61" s="1">
+        <f>C61/B61</f>
+        <v>0.40932345206789383</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62">
+        <v>1236568</v>
+      </c>
+      <c r="C62">
+        <v>507754</v>
+      </c>
+      <c r="D62" s="5" t="str">
+        <f>RIGHT(A62,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E62" s="1">
+        <f>C62/B62</f>
+        <v>0.41061551002451946</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>45</v>
+      </c>
+      <c r="B63">
+        <v>453740</v>
+      </c>
+      <c r="C63">
+        <v>194150</v>
+      </c>
+      <c r="D63" s="5" t="str">
+        <f>RIGHT(A63,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E63" s="1">
+        <f>C63/B63</f>
+        <v>0.42788821792215809</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64">
+        <v>143856</v>
+      </c>
+      <c r="C64">
+        <v>62041</v>
+      </c>
+      <c r="D64" s="5" t="str">
+        <f>RIGHT(A64,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E64" s="1">
+        <f>C64/B64</f>
+        <v>0.43127154932710488</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B65" s="6">
+        <v>421534</v>
+      </c>
+      <c r="C65" s="6">
+        <v>186847</v>
+      </c>
+      <c r="D65" s="5" t="str">
+        <f>RIGHT(A65,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E65" s="1">
+        <f>C65/B65</f>
+        <v>0.44325487386545331</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66">
+        <v>1164813</v>
+      </c>
+      <c r="C66">
+        <v>534807</v>
+      </c>
+      <c r="D66" s="5" t="str">
+        <f>RIGHT(A66,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E66" s="1">
+        <f>C66/B66</f>
+        <v>0.45913550071985804</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>29</v>
+      </c>
+      <c r="B67">
+        <v>146028</v>
+      </c>
+      <c r="C67">
+        <v>67593</v>
+      </c>
+      <c r="D67" s="5" t="str">
+        <f>RIGHT(A67,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E67" s="1">
+        <f>C67/B67</f>
+        <v>0.46287698249650749</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68">
+        <v>147816</v>
+      </c>
+      <c r="C68">
+        <v>69922</v>
+      </c>
+      <c r="D68" s="5" t="str">
+        <f>RIGHT(A68,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E68" s="1">
+        <f>C68/B68</f>
+        <v>0.47303404232288793</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>51</v>
+      </c>
+      <c r="B69">
+        <v>4222419</v>
+      </c>
+      <c r="C69">
+        <v>2018199</v>
+      </c>
+      <c r="D69" s="5" t="str">
+        <f>RIGHT(A69,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E69" s="1">
+        <f>C69/B69</f>
+        <v>0.4779722239787193</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70">
+        <v>433723</v>
+      </c>
+      <c r="C70">
+        <v>211545</v>
+      </c>
+      <c r="D70" s="5" t="str">
+        <f>RIGHT(A70,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E70" s="1">
+        <f>C70/B70</f>
+        <v>0.48774217645824641</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>33</v>
+      </c>
+      <c r="B71">
+        <v>471610</v>
+      </c>
+      <c r="C71">
+        <v>238069</v>
+      </c>
+      <c r="D71" s="5" t="str">
+        <f>RIGHT(A71,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E71" s="1">
+        <f>C71/B71</f>
+        <v>0.50480057674773648</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>69</v>
+      </c>
+      <c r="B72">
+        <v>3881066</v>
+      </c>
+      <c r="C72">
+        <v>2074389</v>
+      </c>
+      <c r="D72" s="5" t="str">
+        <f>RIGHT(A72,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E72" s="1">
+        <f>C72/B72</f>
+        <v>0.53448949335053819</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73">
+        <v>361228</v>
+      </c>
+      <c r="C73">
+        <v>220292</v>
+      </c>
+      <c r="D73" s="5" t="str">
+        <f>RIGHT(A73,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E73" s="1">
+        <f>C73/B73</f>
         <v>0.60984198345643192</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="2">
-        <f>SUM(B2:B49)</f>
-        <v>44533985</v>
-      </c>
-      <c r="C50" s="2">
-        <f>SUM(C2:C49)</f>
-        <v>10096750</v>
-      </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="3">
-        <f>C50/B50</f>
-        <v>0.22672011049538909</v>
+    <row r="74" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="2">
+        <f>SUM(B2:B73)</f>
+        <v>53468676</v>
+      </c>
+      <c r="C74" s="2">
+        <f>SUM(C2:C73)</f>
+        <v>13923472</v>
+      </c>
+      <c r="D74" s="4"/>
+      <c r="E74" s="3">
+        <f>C74/B74</f>
+        <v>0.26040427857237386</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E51">
-    <sortCondition ref="D2:D51"/>
-    <sortCondition ref="E2:E51"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E76">
+    <sortCondition ref="D2:D76"/>
+    <sortCondition ref="E2:E76"/>
   </sortState>
   <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
Image compressed. Statistics about image compression.
</commit_message>
<xml_diff>
--- a/assets/savedSpaceByImageCompression.xlsx
+++ b/assets/savedSpaceByImageCompression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Elephant/Users/uwe/Documents/BC-projects/Development/html/EO4SD Dissemination Platform/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D84369-DCC2-4742-82F3-4F6F03D438E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199F021F-DE5C-C14D-B768-D351FF0D49D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5500" windowWidth="28040" windowHeight="21460" xr2:uid="{719E5152-29F4-104E-98F5-853B818EE6D2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>before</t>
   </si>
@@ -265,16 +265,23 @@
   </si>
   <si>
     <t>images/dummy.png</t>
+  </si>
+  <si>
+    <t>data/BayOfBengal/Myanmar_chla_20200421.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> | Bin  -&gt; </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="[&lt;1000]\ #,##0.00&quot; KB &quot;;[&lt;1000000]#,##0.00,&quot; MB&quot;;#,##0.00,,&quot; GB&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -289,6 +296,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFF7F7F7"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -311,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -323,6 +337,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -637,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D806A48-ED72-0849-8E9A-12CEF63F99B8}">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,13 +684,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="B2">
-        <v>121818</v>
+        <v>3158456</v>
       </c>
       <c r="C2">
-        <v>13002</v>
+        <v>276804</v>
       </c>
       <c r="D2" s="5" t="str">
         <f>RIGHT(A2,3)</f>
@@ -682,18 +698,18 @@
       </c>
       <c r="E2" s="1">
         <f>C2/B2</f>
-        <v>0.10673299512387333</v>
+        <v>8.7639023624201187E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B3">
-        <v>158133</v>
+        <v>121818</v>
       </c>
       <c r="C3">
-        <v>17029</v>
+        <v>13002</v>
       </c>
       <c r="D3" s="5" t="str">
         <f>RIGHT(A3,3)</f>
@@ -701,18 +717,18 @@
       </c>
       <c r="E3" s="1">
         <f>C3/B3</f>
-        <v>0.10768783239425041</v>
+        <v>0.10673299512387333</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B4">
-        <v>273993</v>
+        <v>158133</v>
       </c>
       <c r="C4">
-        <v>29674</v>
+        <v>17029</v>
       </c>
       <c r="D4" s="5" t="str">
         <f>RIGHT(A4,3)</f>
@@ -720,18 +736,18 @@
       </c>
       <c r="E4" s="1">
         <f>C4/B4</f>
-        <v>0.1083020369133518</v>
+        <v>0.10768783239425041</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B5">
-        <v>2620661</v>
+        <v>273993</v>
       </c>
       <c r="C5">
-        <v>286920</v>
+        <v>29674</v>
       </c>
       <c r="D5" s="5" t="str">
         <f>RIGHT(A5,3)</f>
@@ -739,18 +755,18 @@
       </c>
       <c r="E5" s="1">
         <f>C5/B5</f>
-        <v>0.10948382869817957</v>
+        <v>0.1083020369133518</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B6">
-        <v>537820</v>
+        <v>2620661</v>
       </c>
       <c r="C6">
-        <v>60194</v>
+        <v>286920</v>
       </c>
       <c r="D6" s="5" t="str">
         <f>RIGHT(A6,3)</f>
@@ -758,18 +774,18 @@
       </c>
       <c r="E6" s="1">
         <f>C6/B6</f>
-        <v>0.11192220445502213</v>
+        <v>0.10948382869817957</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B7">
-        <v>177913</v>
+        <v>537820</v>
       </c>
       <c r="C7">
-        <v>20041</v>
+        <v>60194</v>
       </c>
       <c r="D7" s="5" t="str">
         <f>RIGHT(A7,3)</f>
@@ -777,18 +793,18 @@
       </c>
       <c r="E7" s="1">
         <f>C7/B7</f>
-        <v>0.11264494443913599</v>
+        <v>0.11192220445502213</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B8">
-        <v>1458872</v>
+        <v>177913</v>
       </c>
       <c r="C8">
-        <v>172179</v>
+        <v>20041</v>
       </c>
       <c r="D8" s="5" t="str">
         <f>RIGHT(A8,3)</f>
@@ -796,18 +812,18 @@
       </c>
       <c r="E8" s="1">
         <f>C8/B8</f>
-        <v>0.11802200604302503</v>
+        <v>0.11264494443913599</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B9">
-        <v>1593763</v>
+        <v>1458872</v>
       </c>
       <c r="C9">
-        <v>190088</v>
+        <v>172179</v>
       </c>
       <c r="D9" s="5" t="str">
         <f>RIGHT(A9,3)</f>
@@ -815,18 +831,18 @@
       </c>
       <c r="E9" s="1">
         <f>C9/B9</f>
-        <v>0.11926992909234309</v>
+        <v>0.11802200604302503</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B10">
-        <v>3031465</v>
+        <v>1593763</v>
       </c>
       <c r="C10">
-        <v>369405</v>
+        <v>190088</v>
       </c>
       <c r="D10" s="5" t="str">
         <f>RIGHT(A10,3)</f>
@@ -834,18 +850,18 @@
       </c>
       <c r="E10" s="1">
         <f>C10/B10</f>
-        <v>0.12185692396250658</v>
+        <v>0.11926992909234309</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B11">
-        <v>110072</v>
+        <v>3031465</v>
       </c>
       <c r="C11">
-        <v>13743</v>
+        <v>369405</v>
       </c>
       <c r="D11" s="5" t="str">
         <f>RIGHT(A11,3)</f>
@@ -853,18 +869,18 @@
       </c>
       <c r="E11" s="1">
         <f>C11/B11</f>
-        <v>0.12485464059888074</v>
+        <v>0.12185692396250658</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <v>201822</v>
+        <v>110072</v>
       </c>
       <c r="C12">
-        <v>25831</v>
+        <v>13743</v>
       </c>
       <c r="D12" s="5" t="str">
         <f>RIGHT(A12,3)</f>
@@ -872,18 +888,18 @@
       </c>
       <c r="E12" s="1">
         <f>C12/B12</f>
-        <v>0.12798902002754903</v>
+        <v>0.12485464059888074</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B13">
-        <v>141078</v>
+        <v>201822</v>
       </c>
       <c r="C13">
-        <v>18511</v>
+        <v>25831</v>
       </c>
       <c r="D13" s="5" t="str">
         <f>RIGHT(A13,3)</f>
@@ -891,18 +907,18 @@
       </c>
       <c r="E13" s="1">
         <f>C13/B13</f>
-        <v>0.13121110307773004</v>
+        <v>0.12798902002754903</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B14">
-        <v>3883376</v>
+        <v>141078</v>
       </c>
       <c r="C14">
-        <v>510382</v>
+        <v>18511</v>
       </c>
       <c r="D14" s="5" t="str">
         <f>RIGHT(A14,3)</f>
@@ -910,18 +926,18 @@
       </c>
       <c r="E14" s="1">
         <f>C14/B14</f>
-        <v>0.13142739719254587</v>
+        <v>0.13121110307773004</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="B15">
-        <v>170997</v>
+        <v>3883376</v>
       </c>
       <c r="C15">
-        <v>22543</v>
+        <v>510382</v>
       </c>
       <c r="D15" s="5" t="str">
         <f>RIGHT(A15,3)</f>
@@ -929,18 +945,18 @@
       </c>
       <c r="E15" s="1">
         <f>C15/B15</f>
-        <v>0.13183272221150077</v>
+        <v>0.13142739719254587</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B16">
-        <v>156551</v>
+        <v>170997</v>
       </c>
       <c r="C16">
-        <v>20743</v>
+        <v>22543</v>
       </c>
       <c r="D16" s="5" t="str">
         <f>RIGHT(A16,3)</f>
@@ -948,18 +964,18 @@
       </c>
       <c r="E16" s="1">
         <f>C16/B16</f>
-        <v>0.1324999520922894</v>
+        <v>0.13183272221150077</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B17">
-        <v>6014206</v>
+        <v>156551</v>
       </c>
       <c r="C17">
-        <v>866156</v>
+        <v>20743</v>
       </c>
       <c r="D17" s="5" t="str">
         <f>RIGHT(A17,3)</f>
@@ -967,18 +983,18 @@
       </c>
       <c r="E17" s="1">
         <f>C17/B17</f>
-        <v>0.14401834589636603</v>
+        <v>0.1324999520922894</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B18">
-        <v>118069</v>
+        <v>6014206</v>
       </c>
       <c r="C18">
-        <v>17465</v>
+        <v>866156</v>
       </c>
       <c r="D18" s="5" t="str">
         <f>RIGHT(A18,3)</f>
@@ -986,18 +1002,18 @@
       </c>
       <c r="E18" s="1">
         <f>C18/B18</f>
-        <v>0.14792197782652516</v>
+        <v>0.14401834589636603</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B19">
-        <v>270341</v>
+        <v>118069</v>
       </c>
       <c r="C19">
-        <v>40632</v>
+        <v>17465</v>
       </c>
       <c r="D19" s="5" t="str">
         <f>RIGHT(A19,3)</f>
@@ -1005,18 +1021,18 @@
       </c>
       <c r="E19" s="1">
         <f>C19/B19</f>
-        <v>0.15029906673423565</v>
+        <v>0.14792197782652516</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B20">
-        <v>5472452</v>
+        <v>270341</v>
       </c>
       <c r="C20">
-        <v>830966</v>
+        <v>40632</v>
       </c>
       <c r="D20" s="5" t="str">
         <f>RIGHT(A20,3)</f>
@@ -1024,18 +1040,18 @@
       </c>
       <c r="E20" s="1">
         <f>C20/B20</f>
-        <v>0.15184527886219926</v>
+        <v>0.15029906673423565</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B21">
-        <v>3824920</v>
+        <v>5472452</v>
       </c>
       <c r="C21">
-        <v>592220</v>
+        <v>830966</v>
       </c>
       <c r="D21" s="5" t="str">
         <f>RIGHT(A21,3)</f>
@@ -1043,18 +1059,18 @@
       </c>
       <c r="E21" s="1">
         <f>C21/B21</f>
-        <v>0.15483199648620102</v>
+        <v>0.15184527886219926</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="B22">
-        <v>161202</v>
+        <v>3824920</v>
       </c>
       <c r="C22">
-        <v>25263</v>
+        <v>592220</v>
       </c>
       <c r="D22" s="5" t="str">
         <f>RIGHT(A22,3)</f>
@@ -1062,56 +1078,56 @@
       </c>
       <c r="E22" s="1">
         <f>C22/B22</f>
-        <v>0.15671641791044777</v>
+        <v>0.15483199648620102</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B23">
-        <v>216625</v>
+        <v>161202</v>
       </c>
       <c r="C23">
-        <v>40653</v>
+        <v>25263</v>
       </c>
       <c r="D23" s="5" t="str">
         <f>RIGHT(A23,3)</f>
-        <v>JPG</v>
+        <v>jpg</v>
       </c>
       <c r="E23" s="1">
         <f>C23/B23</f>
-        <v>0.18766532025389498</v>
+        <v>0.15671641791044777</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B24">
-        <v>180997</v>
+        <v>216625</v>
       </c>
       <c r="C24">
-        <v>36774</v>
+        <v>40653</v>
       </c>
       <c r="D24" s="5" t="str">
         <f>RIGHT(A24,3)</f>
-        <v>jpg</v>
+        <v>JPG</v>
       </c>
       <c r="E24" s="1">
         <f>C24/B24</f>
-        <v>0.20317463825367271</v>
+        <v>0.18766532025389498</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>315663</v>
+        <v>180997</v>
       </c>
       <c r="C25">
-        <v>65625</v>
+        <v>36774</v>
       </c>
       <c r="D25" s="5" t="str">
         <f>RIGHT(A25,3)</f>
@@ -1119,18 +1135,18 @@
       </c>
       <c r="E25" s="1">
         <f>C25/B25</f>
-        <v>0.20789576225278225</v>
+        <v>0.20317463825367271</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="B26">
-        <v>232566</v>
+        <v>315663</v>
       </c>
       <c r="C26">
-        <v>49686</v>
+        <v>65625</v>
       </c>
       <c r="D26" s="5" t="str">
         <f>RIGHT(A26,3)</f>
@@ -1138,18 +1154,18 @@
       </c>
       <c r="E26" s="1">
         <f>C26/B26</f>
-        <v>0.21364257888083382</v>
+        <v>0.20789576225278225</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B27">
-        <v>249044</v>
+        <v>232566</v>
       </c>
       <c r="C27">
-        <v>55418</v>
+        <v>49686</v>
       </c>
       <c r="D27" s="5" t="str">
         <f>RIGHT(A27,3)</f>
@@ -1157,37 +1173,37 @@
       </c>
       <c r="E27" s="1">
         <f>C27/B27</f>
-        <v>0.22252292767543086</v>
+        <v>0.21364257888083382</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="B28">
-        <v>1303470</v>
+        <v>249044</v>
       </c>
       <c r="C28">
-        <v>382283</v>
+        <v>55418</v>
       </c>
       <c r="D28" s="5" t="str">
         <f>RIGHT(A28,3)</f>
-        <v>png</v>
+        <v>jpg</v>
       </c>
       <c r="E28" s="1">
         <f>C28/B28</f>
-        <v>0.2932810114540419</v>
+        <v>0.22252292767543086</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B29">
-        <v>108835</v>
+        <v>1303470</v>
       </c>
       <c r="C29">
-        <v>32568</v>
+        <v>382283</v>
       </c>
       <c r="D29" s="5" t="str">
         <f>RIGHT(A29,3)</f>
@@ -1195,37 +1211,37 @@
       </c>
       <c r="E29" s="1">
         <f>C29/B29</f>
-        <v>0.29924197179216244</v>
+        <v>0.2932810114540419</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B30">
-        <v>48327</v>
+        <v>108835</v>
       </c>
       <c r="C30">
-        <v>14517</v>
+        <v>32568</v>
       </c>
       <c r="D30" s="5" t="str">
         <f>RIGHT(A30,3)</f>
-        <v>PNG</v>
+        <v>png</v>
       </c>
       <c r="E30" s="1">
         <f>C30/B30</f>
-        <v>0.30039108572847478</v>
+        <v>0.29924197179216244</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B31">
-        <v>42125</v>
+        <v>48327</v>
       </c>
       <c r="C31">
-        <v>12974</v>
+        <v>14517</v>
       </c>
       <c r="D31" s="5" t="str">
         <f>RIGHT(A31,3)</f>
@@ -1233,18 +1249,18 @@
       </c>
       <c r="E31" s="1">
         <f>C31/B31</f>
-        <v>0.3079881305637982</v>
+        <v>0.30039108572847478</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B32">
-        <v>53662</v>
+        <v>42125</v>
       </c>
       <c r="C32">
-        <v>16549</v>
+        <v>12974</v>
       </c>
       <c r="D32" s="5" t="str">
         <f>RIGHT(A32,3)</f>
@@ -1252,75 +1268,75 @@
       </c>
       <c r="E32" s="1">
         <f>C32/B32</f>
-        <v>0.30839327643397563</v>
+        <v>0.3079881305637982</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B33">
-        <v>31131</v>
+        <v>53662</v>
       </c>
       <c r="C33">
-        <v>9638</v>
+        <v>16549</v>
       </c>
       <c r="D33" s="5" t="str">
         <f>RIGHT(A33,3)</f>
-        <v>png</v>
+        <v>PNG</v>
       </c>
       <c r="E33" s="1">
         <f>C33/B33</f>
-        <v>0.30959493752208411</v>
+        <v>0.30839327643397563</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B34">
-        <v>53851</v>
+        <v>31131</v>
       </c>
       <c r="C34">
-        <v>16739</v>
+        <v>9638</v>
       </c>
       <c r="D34" s="5" t="str">
         <f>RIGHT(A34,3)</f>
-        <v>PNG</v>
+        <v>png</v>
       </c>
       <c r="E34" s="1">
         <f>C34/B34</f>
-        <v>0.31083916733208294</v>
+        <v>0.30959493752208411</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B35">
-        <v>45078</v>
+        <v>53851</v>
       </c>
       <c r="C35">
-        <v>14098</v>
+        <v>16739</v>
       </c>
       <c r="D35" s="5" t="str">
         <f>RIGHT(A35,3)</f>
-        <v>png</v>
+        <v>PNG</v>
       </c>
       <c r="E35" s="1">
         <f>C35/B35</f>
-        <v>0.31274679444518388</v>
+        <v>0.31083916733208294</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B36">
-        <v>251396</v>
+        <v>45078</v>
       </c>
       <c r="C36">
-        <v>81297</v>
+        <v>14098</v>
       </c>
       <c r="D36" s="5" t="str">
         <f>RIGHT(A36,3)</f>
@@ -1328,18 +1344,18 @@
       </c>
       <c r="E36" s="1">
         <f>C36/B36</f>
-        <v>0.32338223360753554</v>
+        <v>0.31274679444518388</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B37">
-        <v>46405</v>
+        <v>251396</v>
       </c>
       <c r="C37">
-        <v>15561</v>
+        <v>81297</v>
       </c>
       <c r="D37" s="5" t="str">
         <f>RIGHT(A37,3)</f>
@@ -1347,18 +1363,18 @@
       </c>
       <c r="E37" s="1">
         <f>C37/B37</f>
-        <v>0.33533024458571276</v>
+        <v>0.32338223360753554</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B38">
-        <v>43435</v>
+        <v>46405</v>
       </c>
       <c r="C38">
-        <v>14669</v>
+        <v>15561</v>
       </c>
       <c r="D38" s="5" t="str">
         <f>RIGHT(A38,3)</f>
@@ -1366,18 +1382,18 @@
       </c>
       <c r="E38" s="1">
         <f>C38/B38</f>
-        <v>0.33772303441924717</v>
+        <v>0.33533024458571276</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="B39">
-        <v>129963</v>
+        <v>43435</v>
       </c>
       <c r="C39">
-        <v>44568</v>
+        <v>14669</v>
       </c>
       <c r="D39" s="5" t="str">
         <f>RIGHT(A39,3)</f>
@@ -1385,18 +1401,18 @@
       </c>
       <c r="E39" s="1">
         <f>C39/B39</f>
-        <v>0.34292837192123909</v>
+        <v>0.33772303441924717</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="B40">
-        <v>27647</v>
+        <v>129963</v>
       </c>
       <c r="C40">
-        <v>9649</v>
+        <v>44568</v>
       </c>
       <c r="D40" s="5" t="str">
         <f>RIGHT(A40,3)</f>
@@ -1404,18 +1420,18 @@
       </c>
       <c r="E40" s="1">
         <f>C40/B40</f>
-        <v>0.34900712554707564</v>
+        <v>0.34292837192123909</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="B41">
-        <v>38323</v>
+        <v>27647</v>
       </c>
       <c r="C41">
-        <v>13404</v>
+        <v>9649</v>
       </c>
       <c r="D41" s="5" t="str">
         <f>RIGHT(A41,3)</f>
@@ -1423,18 +1439,18 @@
       </c>
       <c r="E41" s="1">
         <f>C41/B41</f>
-        <v>0.34976384938548655</v>
+        <v>0.34900712554707564</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B42">
-        <v>71958</v>
+        <v>38323</v>
       </c>
       <c r="C42">
-        <v>25463</v>
+        <v>13404</v>
       </c>
       <c r="D42" s="5" t="str">
         <f>RIGHT(A42,3)</f>
@@ -1442,18 +1458,18 @@
       </c>
       <c r="E42" s="1">
         <f>C42/B42</f>
-        <v>0.35385919564190221</v>
+        <v>0.34976384938548655</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B43">
-        <v>104911</v>
+        <v>71958</v>
       </c>
       <c r="C43">
-        <v>37368</v>
+        <v>25463</v>
       </c>
       <c r="D43" s="5" t="str">
         <f>RIGHT(A43,3)</f>
@@ -1461,18 +1477,18 @@
       </c>
       <c r="E43" s="1">
         <f>C43/B43</f>
-        <v>0.3561876257017853</v>
+        <v>0.35385919564190221</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B44">
-        <v>592813</v>
+        <v>104911</v>
       </c>
       <c r="C44">
-        <v>214113</v>
+        <v>37368</v>
       </c>
       <c r="D44" s="5" t="str">
         <f>RIGHT(A44,3)</f>
@@ -1480,18 +1496,18 @@
       </c>
       <c r="E44" s="1">
         <f>C44/B44</f>
-        <v>0.36118135061140699</v>
+        <v>0.3561876257017853</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B45">
-        <v>99320</v>
+        <v>592813</v>
       </c>
       <c r="C45">
-        <v>36047</v>
+        <v>214113</v>
       </c>
       <c r="D45" s="5" t="str">
         <f>RIGHT(A45,3)</f>
@@ -1499,18 +1515,18 @@
       </c>
       <c r="E45" s="1">
         <f>C45/B45</f>
-        <v>0.36293797825211438</v>
+        <v>0.36118135061140699</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B46">
-        <v>732692</v>
+        <v>99320</v>
       </c>
       <c r="C46">
-        <v>270414</v>
+        <v>36047</v>
       </c>
       <c r="D46" s="5" t="str">
         <f>RIGHT(A46,3)</f>
@@ -1518,18 +1534,18 @@
       </c>
       <c r="E46" s="1">
         <f>C46/B46</f>
-        <v>0.36906913136761421</v>
+        <v>0.36293797825211438</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B47">
-        <v>596140</v>
+        <v>732692</v>
       </c>
       <c r="C47">
-        <v>220604</v>
+        <v>270414</v>
       </c>
       <c r="D47" s="5" t="str">
         <f>RIGHT(A47,3)</f>
@@ -1537,18 +1553,18 @@
       </c>
       <c r="E47" s="1">
         <f>C47/B47</f>
-        <v>0.37005401415774819</v>
+        <v>0.36906913136761421</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B48">
-        <v>38892</v>
+        <v>596140</v>
       </c>
       <c r="C48">
-        <v>14531</v>
+        <v>220604</v>
       </c>
       <c r="D48" s="5" t="str">
         <f>RIGHT(A48,3)</f>
@@ -1556,18 +1572,18 @@
       </c>
       <c r="E48" s="1">
         <f>C48/B48</f>
-        <v>0.37362439576262468</v>
+        <v>0.37005401415774819</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B49">
-        <v>37592</v>
+        <v>38892</v>
       </c>
       <c r="C49">
-        <v>14080</v>
+        <v>14531</v>
       </c>
       <c r="D49" s="5" t="str">
         <f>RIGHT(A49,3)</f>
@@ -1575,18 +1591,18 @@
       </c>
       <c r="E49" s="1">
         <f>C49/B49</f>
-        <v>0.37454777612257928</v>
+        <v>0.37362439576262468</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B50">
-        <v>794917</v>
+        <v>37592</v>
       </c>
       <c r="C50">
-        <v>300100</v>
+        <v>14080</v>
       </c>
       <c r="D50" s="5" t="str">
         <f>RIGHT(A50,3)</f>
@@ -1594,18 +1610,18 @@
       </c>
       <c r="E50" s="1">
         <f>C50/B50</f>
-        <v>0.37752369115266121</v>
+        <v>0.37454777612257928</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B51">
-        <v>103718</v>
+        <v>794917</v>
       </c>
       <c r="C51">
-        <v>39559</v>
+        <v>300100</v>
       </c>
       <c r="D51" s="5" t="str">
         <f>RIGHT(A51,3)</f>
@@ -1613,18 +1629,18 @@
       </c>
       <c r="E51" s="1">
         <f>C51/B51</f>
-        <v>0.38140920573092424</v>
+        <v>0.37752369115266121</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B52">
-        <v>607591</v>
+        <v>103718</v>
       </c>
       <c r="C52">
-        <v>232884</v>
+        <v>39559</v>
       </c>
       <c r="D52" s="5" t="str">
         <f>RIGHT(A52,3)</f>
@@ -1632,18 +1648,18 @@
       </c>
       <c r="E52" s="1">
         <f>C52/B52</f>
-        <v>0.3832907334045435</v>
+        <v>0.38140920573092424</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="B53">
-        <v>49352</v>
+        <v>607591</v>
       </c>
       <c r="C53">
-        <v>19054</v>
+        <v>232884</v>
       </c>
       <c r="D53" s="5" t="str">
         <f>RIGHT(A53,3)</f>
@@ -1651,18 +1667,18 @@
       </c>
       <c r="E53" s="1">
         <f>C53/B53</f>
-        <v>0.38608364402658452</v>
+        <v>0.3832907334045435</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B54">
-        <v>362496</v>
+        <v>49352</v>
       </c>
       <c r="C54">
-        <v>140096</v>
+        <v>19054</v>
       </c>
       <c r="D54" s="5" t="str">
         <f>RIGHT(A54,3)</f>
@@ -1670,18 +1686,18 @@
       </c>
       <c r="E54" s="1">
         <f>C54/B54</f>
-        <v>0.38647598870056499</v>
+        <v>0.38608364402658452</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="B55">
-        <v>299628</v>
+        <v>362496</v>
       </c>
       <c r="C55">
-        <v>117140</v>
+        <v>140096</v>
       </c>
       <c r="D55" s="5" t="str">
         <f>RIGHT(A55,3)</f>
@@ -1689,18 +1705,18 @@
       </c>
       <c r="E55" s="1">
         <f>C55/B55</f>
-        <v>0.39095144646027741</v>
+        <v>0.38647598870056499</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="B56">
-        <v>182490</v>
+        <v>299628</v>
       </c>
       <c r="C56">
-        <v>71410</v>
+        <v>117140</v>
       </c>
       <c r="D56" s="5" t="str">
         <f>RIGHT(A56,3)</f>
@@ -1708,18 +1724,18 @@
       </c>
       <c r="E56" s="1">
         <f>C56/B56</f>
-        <v>0.39130911282810016</v>
+        <v>0.39095144646027741</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="B57">
-        <v>1172756</v>
+        <v>182490</v>
       </c>
       <c r="C57">
-        <v>466441</v>
+        <v>71410</v>
       </c>
       <c r="D57" s="5" t="str">
         <f>RIGHT(A57,3)</f>
@@ -1727,18 +1743,18 @@
       </c>
       <c r="E57" s="1">
         <f>C57/B57</f>
-        <v>0.39773064473769482</v>
+        <v>0.39130911282810016</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B58">
-        <v>284286</v>
+        <v>1172756</v>
       </c>
       <c r="C58">
-        <v>113724</v>
+        <v>466441</v>
       </c>
       <c r="D58" s="5" t="str">
         <f>RIGHT(A58,3)</f>
@@ -1746,18 +1762,18 @@
       </c>
       <c r="E58" s="1">
         <f>C58/B58</f>
-        <v>0.40003376881028258</v>
+        <v>0.39773064473769482</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B59">
-        <v>116510</v>
+        <v>284286</v>
       </c>
       <c r="C59">
-        <v>46835</v>
+        <v>113724</v>
       </c>
       <c r="D59" s="5" t="str">
         <f>RIGHT(A59,3)</f>
@@ -1765,18 +1781,18 @@
       </c>
       <c r="E59" s="1">
         <f>C59/B59</f>
-        <v>0.40198266243240921</v>
+        <v>0.40003376881028258</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B60">
-        <v>197231</v>
+        <v>116510</v>
       </c>
       <c r="C60">
-        <v>79783</v>
+        <v>46835</v>
       </c>
       <c r="D60" s="5" t="str">
         <f>RIGHT(A60,3)</f>
@@ -1784,18 +1800,18 @@
       </c>
       <c r="E60" s="1">
         <f>C60/B60</f>
-        <v>0.40451551733753821</v>
+        <v>0.40198266243240921</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B61">
-        <v>20915</v>
+        <v>197231</v>
       </c>
       <c r="C61">
-        <v>8561</v>
+        <v>79783</v>
       </c>
       <c r="D61" s="5" t="str">
         <f>RIGHT(A61,3)</f>
@@ -1803,18 +1819,18 @@
       </c>
       <c r="E61" s="1">
         <f>C61/B61</f>
-        <v>0.40932345206789383</v>
+        <v>0.40451551733753821</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="B62">
-        <v>1236568</v>
+        <v>20915</v>
       </c>
       <c r="C62">
-        <v>507754</v>
+        <v>8561</v>
       </c>
       <c r="D62" s="5" t="str">
         <f>RIGHT(A62,3)</f>
@@ -1822,18 +1838,18 @@
       </c>
       <c r="E62" s="1">
         <f>C62/B62</f>
-        <v>0.41061551002451946</v>
+        <v>0.40932345206789383</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B63">
-        <v>453740</v>
+        <v>1236568</v>
       </c>
       <c r="C63">
-        <v>194150</v>
+        <v>507754</v>
       </c>
       <c r="D63" s="5" t="str">
         <f>RIGHT(A63,3)</f>
@@ -1841,18 +1857,18 @@
       </c>
       <c r="E63" s="1">
         <f>C63/B63</f>
-        <v>0.42788821792215809</v>
+        <v>0.41061551002451946</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="B64">
-        <v>143856</v>
+        <v>453740</v>
       </c>
       <c r="C64">
-        <v>62041</v>
+        <v>194150</v>
       </c>
       <c r="D64" s="5" t="str">
         <f>RIGHT(A64,3)</f>
@@ -1860,18 +1876,18 @@
       </c>
       <c r="E64" s="1">
         <f>C64/B64</f>
-        <v>0.43127154932710488</v>
+        <v>0.42788821792215809</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B65" s="6">
-        <v>421534</v>
-      </c>
-      <c r="C65" s="6">
-        <v>186847</v>
+      <c r="A65" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65">
+        <v>143856</v>
+      </c>
+      <c r="C65">
+        <v>62041</v>
       </c>
       <c r="D65" s="5" t="str">
         <f>RIGHT(A65,3)</f>
@@ -1879,18 +1895,18 @@
       </c>
       <c r="E65" s="1">
         <f>C65/B65</f>
-        <v>0.44325487386545331</v>
+        <v>0.43127154932710488</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>10</v>
-      </c>
-      <c r="B66">
-        <v>1164813</v>
-      </c>
-      <c r="C66">
-        <v>534807</v>
+      <c r="A66" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B66" s="6">
+        <v>421534</v>
+      </c>
+      <c r="C66" s="6">
+        <v>186847</v>
       </c>
       <c r="D66" s="5" t="str">
         <f>RIGHT(A66,3)</f>
@@ -1898,18 +1914,18 @@
       </c>
       <c r="E66" s="1">
         <f>C66/B66</f>
-        <v>0.45913550071985804</v>
+        <v>0.44325487386545331</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B67">
-        <v>146028</v>
+        <v>1164813</v>
       </c>
       <c r="C67">
-        <v>67593</v>
+        <v>534807</v>
       </c>
       <c r="D67" s="5" t="str">
         <f>RIGHT(A67,3)</f>
@@ -1917,18 +1933,18 @@
       </c>
       <c r="E67" s="1">
         <f>C67/B67</f>
-        <v>0.46287698249650749</v>
+        <v>0.45913550071985804</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="B68">
-        <v>147816</v>
+        <v>146028</v>
       </c>
       <c r="C68">
-        <v>69922</v>
+        <v>67593</v>
       </c>
       <c r="D68" s="5" t="str">
         <f>RIGHT(A68,3)</f>
@@ -1936,18 +1952,18 @@
       </c>
       <c r="E68" s="1">
         <f>C68/B68</f>
-        <v>0.47303404232288793</v>
+        <v>0.46287698249650749</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="B69">
-        <v>4222419</v>
+        <v>147816</v>
       </c>
       <c r="C69">
-        <v>2018199</v>
+        <v>69922</v>
       </c>
       <c r="D69" s="5" t="str">
         <f>RIGHT(A69,3)</f>
@@ -1955,18 +1971,18 @@
       </c>
       <c r="E69" s="1">
         <f>C69/B69</f>
-        <v>0.4779722239787193</v>
+        <v>0.47303404232288793</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="B70">
-        <v>433723</v>
+        <v>4222419</v>
       </c>
       <c r="C70">
-        <v>211545</v>
+        <v>2018199</v>
       </c>
       <c r="D70" s="5" t="str">
         <f>RIGHT(A70,3)</f>
@@ -1974,18 +1990,18 @@
       </c>
       <c r="E70" s="1">
         <f>C70/B70</f>
-        <v>0.48774217645824641</v>
+        <v>0.4779722239787193</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B71">
-        <v>471610</v>
+        <v>433723</v>
       </c>
       <c r="C71">
-        <v>238069</v>
+        <v>211545</v>
       </c>
       <c r="D71" s="5" t="str">
         <f>RIGHT(A71,3)</f>
@@ -1993,18 +2009,18 @@
       </c>
       <c r="E71" s="1">
         <f>C71/B71</f>
-        <v>0.50480057674773648</v>
+        <v>0.48774217645824641</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B72">
-        <v>3881066</v>
+        <v>471610</v>
       </c>
       <c r="C72">
-        <v>2074389</v>
+        <v>238069</v>
       </c>
       <c r="D72" s="5" t="str">
         <f>RIGHT(A72,3)</f>
@@ -2012,18 +2028,18 @@
       </c>
       <c r="E72" s="1">
         <f>C72/B72</f>
-        <v>0.53448949335053819</v>
+        <v>0.50480057674773648</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B73">
-        <v>361228</v>
+        <v>3881066</v>
       </c>
       <c r="C73">
-        <v>220292</v>
+        <v>2074389</v>
       </c>
       <c r="D73" s="5" t="str">
         <f>RIGHT(A73,3)</f>
@@ -2031,28 +2047,52 @@
       </c>
       <c r="E73" s="1">
         <f>C73/B73</f>
+        <v>0.53448949335053819</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74">
+        <v>361228</v>
+      </c>
+      <c r="C74">
+        <v>220292</v>
+      </c>
+      <c r="D74" s="5" t="str">
+        <f>RIGHT(A74,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E74" s="1">
+        <f>C74/B74</f>
         <v>0.60984198345643192</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="2">
-        <f>SUM(B2:B73)</f>
-        <v>53468676</v>
-      </c>
-      <c r="C74" s="2">
-        <f>SUM(C2:C73)</f>
-        <v>13923472</v>
-      </c>
-      <c r="D74" s="4"/>
-      <c r="E74" s="3">
-        <f>C74/B74</f>
-        <v>0.26040427857237386</v>
+    <row r="75" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="8">
+        <f>SUM(B2:B74)</f>
+        <v>56627132</v>
+      </c>
+      <c r="C75" s="8">
+        <f>SUM(C2:C74)</f>
+        <v>14200276</v>
+      </c>
+      <c r="D75" s="4"/>
+      <c r="E75" s="3">
+        <f>C75/B75</f>
+        <v>0.25076805938185248</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A80" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E76">
-    <sortCondition ref="D2:D76"/>
-    <sortCondition ref="E2:E76"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E81">
+    <sortCondition ref="D2:D81"/>
+    <sortCondition ref="E2:E81"/>
   </sortState>
   <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
Statistics about image compression.
</commit_message>
<xml_diff>
--- a/assets/savedSpaceByImageCompression.xlsx
+++ b/assets/savedSpaceByImageCompression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Elephant/Users/uwe/Documents/BC-projects/Development/html/EO4SD Dissemination Platform/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199F021F-DE5C-C14D-B768-D351FF0D49D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E4101C-D37D-3E40-9DCE-37D22976CA29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5500" windowWidth="28040" windowHeight="21460" xr2:uid="{719E5152-29F4-104E-98F5-853B818EE6D2}"/>
+    <workbookView xWindow="11560" yWindow="5520" windowWidth="28040" windowHeight="21460" xr2:uid="{719E5152-29F4-104E-98F5-853B818EE6D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>before</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t xml:space="preserve"> | Bin  -&gt; </t>
+  </si>
+  <si>
+    <t>jpg</t>
+  </si>
+  <si>
+    <t>data/BayOfBengal/Myanmar_mangrove_and_landuse_map.png</t>
   </si>
 </sst>
 </file>
@@ -279,7 +285,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="[&lt;1000]\ #,##0.00&quot; KB &quot;;[&lt;1000000]#,##0.00,&quot; MB&quot;;#,##0.00,,&quot; GB&quot;"/>
+    <numFmt numFmtId="165" formatCode="[&lt;1000]\ #,##0.00&quot; KB &quot;;[&lt;1000000]#,##0.00,&quot; MB&quot;;#,##0.00,,&quot; GB&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -338,7 +344,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -653,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D806A48-ED72-0849-8E9A-12CEF63F99B8}">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1197,32 +1203,31 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="B29">
-        <v>1303470</v>
+        <v>13284671</v>
       </c>
       <c r="C29">
-        <v>382283</v>
-      </c>
-      <c r="D29" s="5" t="str">
-        <f>RIGHT(A29,3)</f>
-        <v>png</v>
+        <v>3235628</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="E29" s="1">
         <f>C29/B29</f>
-        <v>0.2932810114540419</v>
+        <v>0.24356101856041448</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B30">
-        <v>108835</v>
+        <v>1303470</v>
       </c>
       <c r="C30">
-        <v>32568</v>
+        <v>382283</v>
       </c>
       <c r="D30" s="5" t="str">
         <f>RIGHT(A30,3)</f>
@@ -1230,37 +1235,37 @@
       </c>
       <c r="E30" s="1">
         <f>C30/B30</f>
-        <v>0.29924197179216244</v>
+        <v>0.2932810114540419</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B31">
-        <v>48327</v>
+        <v>108835</v>
       </c>
       <c r="C31">
-        <v>14517</v>
+        <v>32568</v>
       </c>
       <c r="D31" s="5" t="str">
         <f>RIGHT(A31,3)</f>
-        <v>PNG</v>
+        <v>png</v>
       </c>
       <c r="E31" s="1">
         <f>C31/B31</f>
-        <v>0.30039108572847478</v>
+        <v>0.29924197179216244</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B32">
-        <v>42125</v>
+        <v>48327</v>
       </c>
       <c r="C32">
-        <v>12974</v>
+        <v>14517</v>
       </c>
       <c r="D32" s="5" t="str">
         <f>RIGHT(A32,3)</f>
@@ -1268,18 +1273,18 @@
       </c>
       <c r="E32" s="1">
         <f>C32/B32</f>
-        <v>0.3079881305637982</v>
+        <v>0.30039108572847478</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33">
-        <v>53662</v>
+        <v>42125</v>
       </c>
       <c r="C33">
-        <v>16549</v>
+        <v>12974</v>
       </c>
       <c r="D33" s="5" t="str">
         <f>RIGHT(A33,3)</f>
@@ -1287,75 +1292,75 @@
       </c>
       <c r="E33" s="1">
         <f>C33/B33</f>
-        <v>0.30839327643397563</v>
+        <v>0.3079881305637982</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B34">
-        <v>31131</v>
+        <v>53662</v>
       </c>
       <c r="C34">
-        <v>9638</v>
+        <v>16549</v>
       </c>
       <c r="D34" s="5" t="str">
         <f>RIGHT(A34,3)</f>
-        <v>png</v>
+        <v>PNG</v>
       </c>
       <c r="E34" s="1">
         <f>C34/B34</f>
-        <v>0.30959493752208411</v>
+        <v>0.30839327643397563</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B35">
-        <v>53851</v>
+        <v>31131</v>
       </c>
       <c r="C35">
-        <v>16739</v>
+        <v>9638</v>
       </c>
       <c r="D35" s="5" t="str">
         <f>RIGHT(A35,3)</f>
-        <v>PNG</v>
+        <v>png</v>
       </c>
       <c r="E35" s="1">
         <f>C35/B35</f>
-        <v>0.31083916733208294</v>
+        <v>0.30959493752208411</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B36">
-        <v>45078</v>
+        <v>53851</v>
       </c>
       <c r="C36">
-        <v>14098</v>
+        <v>16739</v>
       </c>
       <c r="D36" s="5" t="str">
         <f>RIGHT(A36,3)</f>
-        <v>png</v>
+        <v>PNG</v>
       </c>
       <c r="E36" s="1">
         <f>C36/B36</f>
-        <v>0.31274679444518388</v>
+        <v>0.31083916733208294</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B37">
-        <v>251396</v>
+        <v>45078</v>
       </c>
       <c r="C37">
-        <v>81297</v>
+        <v>14098</v>
       </c>
       <c r="D37" s="5" t="str">
         <f>RIGHT(A37,3)</f>
@@ -1363,18 +1368,18 @@
       </c>
       <c r="E37" s="1">
         <f>C37/B37</f>
-        <v>0.32338223360753554</v>
+        <v>0.31274679444518388</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38">
-        <v>46405</v>
+        <v>251396</v>
       </c>
       <c r="C38">
-        <v>15561</v>
+        <v>81297</v>
       </c>
       <c r="D38" s="5" t="str">
         <f>RIGHT(A38,3)</f>
@@ -1382,18 +1387,18 @@
       </c>
       <c r="E38" s="1">
         <f>C38/B38</f>
-        <v>0.33533024458571276</v>
+        <v>0.32338223360753554</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B39">
-        <v>43435</v>
+        <v>46405</v>
       </c>
       <c r="C39">
-        <v>14669</v>
+        <v>15561</v>
       </c>
       <c r="D39" s="5" t="str">
         <f>RIGHT(A39,3)</f>
@@ -1401,18 +1406,18 @@
       </c>
       <c r="E39" s="1">
         <f>C39/B39</f>
-        <v>0.33772303441924717</v>
+        <v>0.33533024458571276</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="B40">
-        <v>129963</v>
+        <v>43435</v>
       </c>
       <c r="C40">
-        <v>44568</v>
+        <v>14669</v>
       </c>
       <c r="D40" s="5" t="str">
         <f>RIGHT(A40,3)</f>
@@ -1420,18 +1425,18 @@
       </c>
       <c r="E40" s="1">
         <f>C40/B40</f>
-        <v>0.34292837192123909</v>
+        <v>0.33772303441924717</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="B41">
-        <v>27647</v>
+        <v>129963</v>
       </c>
       <c r="C41">
-        <v>9649</v>
+        <v>44568</v>
       </c>
       <c r="D41" s="5" t="str">
         <f>RIGHT(A41,3)</f>
@@ -1439,18 +1444,18 @@
       </c>
       <c r="E41" s="1">
         <f>C41/B41</f>
-        <v>0.34900712554707564</v>
+        <v>0.34292837192123909</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="B42">
-        <v>38323</v>
+        <v>27647</v>
       </c>
       <c r="C42">
-        <v>13404</v>
+        <v>9649</v>
       </c>
       <c r="D42" s="5" t="str">
         <f>RIGHT(A42,3)</f>
@@ -1458,18 +1463,18 @@
       </c>
       <c r="E42" s="1">
         <f>C42/B42</f>
-        <v>0.34976384938548655</v>
+        <v>0.34900712554707564</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B43">
-        <v>71958</v>
+        <v>38323</v>
       </c>
       <c r="C43">
-        <v>25463</v>
+        <v>13404</v>
       </c>
       <c r="D43" s="5" t="str">
         <f>RIGHT(A43,3)</f>
@@ -1477,18 +1482,18 @@
       </c>
       <c r="E43" s="1">
         <f>C43/B43</f>
-        <v>0.35385919564190221</v>
+        <v>0.34976384938548655</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B44">
-        <v>104911</v>
+        <v>71958</v>
       </c>
       <c r="C44">
-        <v>37368</v>
+        <v>25463</v>
       </c>
       <c r="D44" s="5" t="str">
         <f>RIGHT(A44,3)</f>
@@ -1496,18 +1501,18 @@
       </c>
       <c r="E44" s="1">
         <f>C44/B44</f>
-        <v>0.3561876257017853</v>
+        <v>0.35385919564190221</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B45">
-        <v>592813</v>
+        <v>104911</v>
       </c>
       <c r="C45">
-        <v>214113</v>
+        <v>37368</v>
       </c>
       <c r="D45" s="5" t="str">
         <f>RIGHT(A45,3)</f>
@@ -1515,18 +1520,18 @@
       </c>
       <c r="E45" s="1">
         <f>C45/B45</f>
-        <v>0.36118135061140699</v>
+        <v>0.3561876257017853</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B46">
-        <v>99320</v>
+        <v>592813</v>
       </c>
       <c r="C46">
-        <v>36047</v>
+        <v>214113</v>
       </c>
       <c r="D46" s="5" t="str">
         <f>RIGHT(A46,3)</f>
@@ -1534,18 +1539,18 @@
       </c>
       <c r="E46" s="1">
         <f>C46/B46</f>
-        <v>0.36293797825211438</v>
+        <v>0.36118135061140699</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B47">
-        <v>732692</v>
+        <v>99320</v>
       </c>
       <c r="C47">
-        <v>270414</v>
+        <v>36047</v>
       </c>
       <c r="D47" s="5" t="str">
         <f>RIGHT(A47,3)</f>
@@ -1553,18 +1558,18 @@
       </c>
       <c r="E47" s="1">
         <f>C47/B47</f>
-        <v>0.36906913136761421</v>
+        <v>0.36293797825211438</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B48">
-        <v>596140</v>
+        <v>732692</v>
       </c>
       <c r="C48">
-        <v>220604</v>
+        <v>270414</v>
       </c>
       <c r="D48" s="5" t="str">
         <f>RIGHT(A48,3)</f>
@@ -1572,18 +1577,18 @@
       </c>
       <c r="E48" s="1">
         <f>C48/B48</f>
-        <v>0.37005401415774819</v>
+        <v>0.36906913136761421</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B49">
-        <v>38892</v>
+        <v>596140</v>
       </c>
       <c r="C49">
-        <v>14531</v>
+        <v>220604</v>
       </c>
       <c r="D49" s="5" t="str">
         <f>RIGHT(A49,3)</f>
@@ -1591,18 +1596,18 @@
       </c>
       <c r="E49" s="1">
         <f>C49/B49</f>
-        <v>0.37362439576262468</v>
+        <v>0.37005401415774819</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B50">
-        <v>37592</v>
+        <v>38892</v>
       </c>
       <c r="C50">
-        <v>14080</v>
+        <v>14531</v>
       </c>
       <c r="D50" s="5" t="str">
         <f>RIGHT(A50,3)</f>
@@ -1610,18 +1615,18 @@
       </c>
       <c r="E50" s="1">
         <f>C50/B50</f>
-        <v>0.37454777612257928</v>
+        <v>0.37362439576262468</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B51">
-        <v>794917</v>
+        <v>37592</v>
       </c>
       <c r="C51">
-        <v>300100</v>
+        <v>14080</v>
       </c>
       <c r="D51" s="5" t="str">
         <f>RIGHT(A51,3)</f>
@@ -1629,18 +1634,18 @@
       </c>
       <c r="E51" s="1">
         <f>C51/B51</f>
-        <v>0.37752369115266121</v>
+        <v>0.37454777612257928</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B52">
-        <v>103718</v>
+        <v>794917</v>
       </c>
       <c r="C52">
-        <v>39559</v>
+        <v>300100</v>
       </c>
       <c r="D52" s="5" t="str">
         <f>RIGHT(A52,3)</f>
@@ -1648,18 +1653,18 @@
       </c>
       <c r="E52" s="1">
         <f>C52/B52</f>
-        <v>0.38140920573092424</v>
+        <v>0.37752369115266121</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B53">
-        <v>607591</v>
+        <v>103718</v>
       </c>
       <c r="C53">
-        <v>232884</v>
+        <v>39559</v>
       </c>
       <c r="D53" s="5" t="str">
         <f>RIGHT(A53,3)</f>
@@ -1667,18 +1672,18 @@
       </c>
       <c r="E53" s="1">
         <f>C53/B53</f>
-        <v>0.3832907334045435</v>
+        <v>0.38140920573092424</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="B54">
-        <v>49352</v>
+        <v>607591</v>
       </c>
       <c r="C54">
-        <v>19054</v>
+        <v>232884</v>
       </c>
       <c r="D54" s="5" t="str">
         <f>RIGHT(A54,3)</f>
@@ -1686,18 +1691,18 @@
       </c>
       <c r="E54" s="1">
         <f>C54/B54</f>
-        <v>0.38608364402658452</v>
+        <v>0.3832907334045435</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B55">
-        <v>362496</v>
+        <v>49352</v>
       </c>
       <c r="C55">
-        <v>140096</v>
+        <v>19054</v>
       </c>
       <c r="D55" s="5" t="str">
         <f>RIGHT(A55,3)</f>
@@ -1705,18 +1710,18 @@
       </c>
       <c r="E55" s="1">
         <f>C55/B55</f>
-        <v>0.38647598870056499</v>
+        <v>0.38608364402658452</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="B56">
-        <v>299628</v>
+        <v>362496</v>
       </c>
       <c r="C56">
-        <v>117140</v>
+        <v>140096</v>
       </c>
       <c r="D56" s="5" t="str">
         <f>RIGHT(A56,3)</f>
@@ -1724,18 +1729,18 @@
       </c>
       <c r="E56" s="1">
         <f>C56/B56</f>
-        <v>0.39095144646027741</v>
+        <v>0.38647598870056499</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="B57">
-        <v>182490</v>
+        <v>299628</v>
       </c>
       <c r="C57">
-        <v>71410</v>
+        <v>117140</v>
       </c>
       <c r="D57" s="5" t="str">
         <f>RIGHT(A57,3)</f>
@@ -1743,18 +1748,18 @@
       </c>
       <c r="E57" s="1">
         <f>C57/B57</f>
-        <v>0.39130911282810016</v>
+        <v>0.39095144646027741</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="B58">
-        <v>1172756</v>
+        <v>182490</v>
       </c>
       <c r="C58">
-        <v>466441</v>
+        <v>71410</v>
       </c>
       <c r="D58" s="5" t="str">
         <f>RIGHT(A58,3)</f>
@@ -1762,18 +1767,18 @@
       </c>
       <c r="E58" s="1">
         <f>C58/B58</f>
-        <v>0.39773064473769482</v>
+        <v>0.39130911282810016</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B59">
-        <v>284286</v>
+        <v>1172756</v>
       </c>
       <c r="C59">
-        <v>113724</v>
+        <v>466441</v>
       </c>
       <c r="D59" s="5" t="str">
         <f>RIGHT(A59,3)</f>
@@ -1781,18 +1786,18 @@
       </c>
       <c r="E59" s="1">
         <f>C59/B59</f>
-        <v>0.40003376881028258</v>
+        <v>0.39773064473769482</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B60">
-        <v>116510</v>
+        <v>284286</v>
       </c>
       <c r="C60">
-        <v>46835</v>
+        <v>113724</v>
       </c>
       <c r="D60" s="5" t="str">
         <f>RIGHT(A60,3)</f>
@@ -1800,18 +1805,18 @@
       </c>
       <c r="E60" s="1">
         <f>C60/B60</f>
-        <v>0.40198266243240921</v>
+        <v>0.40003376881028258</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B61">
-        <v>197231</v>
+        <v>116510</v>
       </c>
       <c r="C61">
-        <v>79783</v>
+        <v>46835</v>
       </c>
       <c r="D61" s="5" t="str">
         <f>RIGHT(A61,3)</f>
@@ -1819,18 +1824,18 @@
       </c>
       <c r="E61" s="1">
         <f>C61/B61</f>
-        <v>0.40451551733753821</v>
+        <v>0.40198266243240921</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B62">
-        <v>20915</v>
+        <v>197231</v>
       </c>
       <c r="C62">
-        <v>8561</v>
+        <v>79783</v>
       </c>
       <c r="D62" s="5" t="str">
         <f>RIGHT(A62,3)</f>
@@ -1838,18 +1843,18 @@
       </c>
       <c r="E62" s="1">
         <f>C62/B62</f>
-        <v>0.40932345206789383</v>
+        <v>0.40451551733753821</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="B63">
-        <v>1236568</v>
+        <v>20915</v>
       </c>
       <c r="C63">
-        <v>507754</v>
+        <v>8561</v>
       </c>
       <c r="D63" s="5" t="str">
         <f>RIGHT(A63,3)</f>
@@ -1857,18 +1862,18 @@
       </c>
       <c r="E63" s="1">
         <f>C63/B63</f>
-        <v>0.41061551002451946</v>
+        <v>0.40932345206789383</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B64">
-        <v>453740</v>
+        <v>1236568</v>
       </c>
       <c r="C64">
-        <v>194150</v>
+        <v>507754</v>
       </c>
       <c r="D64" s="5" t="str">
         <f>RIGHT(A64,3)</f>
@@ -1876,18 +1881,18 @@
       </c>
       <c r="E64" s="1">
         <f>C64/B64</f>
-        <v>0.42788821792215809</v>
+        <v>0.41061551002451946</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="B65">
-        <v>143856</v>
+        <v>453740</v>
       </c>
       <c r="C65">
-        <v>62041</v>
+        <v>194150</v>
       </c>
       <c r="D65" s="5" t="str">
         <f>RIGHT(A65,3)</f>
@@ -1895,18 +1900,18 @@
       </c>
       <c r="E65" s="1">
         <f>C65/B65</f>
-        <v>0.43127154932710488</v>
+        <v>0.42788821792215809</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66" s="6">
-        <v>421534</v>
-      </c>
-      <c r="C66" s="6">
-        <v>186847</v>
+      <c r="A66" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66">
+        <v>143856</v>
+      </c>
+      <c r="C66">
+        <v>62041</v>
       </c>
       <c r="D66" s="5" t="str">
         <f>RIGHT(A66,3)</f>
@@ -1914,18 +1919,18 @@
       </c>
       <c r="E66" s="1">
         <f>C66/B66</f>
-        <v>0.44325487386545331</v>
+        <v>0.43127154932710488</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67">
-        <v>1164813</v>
-      </c>
-      <c r="C67">
-        <v>534807</v>
+      <c r="A67" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B67" s="6">
+        <v>421534</v>
+      </c>
+      <c r="C67" s="6">
+        <v>186847</v>
       </c>
       <c r="D67" s="5" t="str">
         <f>RIGHT(A67,3)</f>
@@ -1933,18 +1938,18 @@
       </c>
       <c r="E67" s="1">
         <f>C67/B67</f>
-        <v>0.45913550071985804</v>
+        <v>0.44325487386545331</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B68">
-        <v>146028</v>
+        <v>1164813</v>
       </c>
       <c r="C68">
-        <v>67593</v>
+        <v>534807</v>
       </c>
       <c r="D68" s="5" t="str">
         <f>RIGHT(A68,3)</f>
@@ -1952,18 +1957,18 @@
       </c>
       <c r="E68" s="1">
         <f>C68/B68</f>
-        <v>0.46287698249650749</v>
+        <v>0.45913550071985804</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="B69">
-        <v>147816</v>
+        <v>146028</v>
       </c>
       <c r="C69">
-        <v>69922</v>
+        <v>67593</v>
       </c>
       <c r="D69" s="5" t="str">
         <f>RIGHT(A69,3)</f>
@@ -1971,18 +1976,18 @@
       </c>
       <c r="E69" s="1">
         <f>C69/B69</f>
-        <v>0.47303404232288793</v>
+        <v>0.46287698249650749</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="B70">
-        <v>4222419</v>
+        <v>147816</v>
       </c>
       <c r="C70">
-        <v>2018199</v>
+        <v>69922</v>
       </c>
       <c r="D70" s="5" t="str">
         <f>RIGHT(A70,3)</f>
@@ -1990,18 +1995,18 @@
       </c>
       <c r="E70" s="1">
         <f>C70/B70</f>
-        <v>0.4779722239787193</v>
+        <v>0.47303404232288793</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="B71">
-        <v>433723</v>
+        <v>4222419</v>
       </c>
       <c r="C71">
-        <v>211545</v>
+        <v>2018199</v>
       </c>
       <c r="D71" s="5" t="str">
         <f>RIGHT(A71,3)</f>
@@ -2009,18 +2014,18 @@
       </c>
       <c r="E71" s="1">
         <f>C71/B71</f>
-        <v>0.48774217645824641</v>
+        <v>0.4779722239787193</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B72">
-        <v>471610</v>
+        <v>433723</v>
       </c>
       <c r="C72">
-        <v>238069</v>
+        <v>211545</v>
       </c>
       <c r="D72" s="5" t="str">
         <f>RIGHT(A72,3)</f>
@@ -2028,18 +2033,18 @@
       </c>
       <c r="E72" s="1">
         <f>C72/B72</f>
-        <v>0.50480057674773648</v>
+        <v>0.48774217645824641</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B73">
-        <v>3881066</v>
+        <v>471610</v>
       </c>
       <c r="C73">
-        <v>2074389</v>
+        <v>238069</v>
       </c>
       <c r="D73" s="5" t="str">
         <f>RIGHT(A73,3)</f>
@@ -2047,18 +2052,18 @@
       </c>
       <c r="E73" s="1">
         <f>C73/B73</f>
-        <v>0.53448949335053819</v>
+        <v>0.50480057674773648</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B74">
-        <v>361228</v>
+        <v>3881066</v>
       </c>
       <c r="C74">
-        <v>220292</v>
+        <v>2074389</v>
       </c>
       <c r="D74" s="5" t="str">
         <f>RIGHT(A74,3)</f>
@@ -2066,33 +2071,52 @@
       </c>
       <c r="E74" s="1">
         <f>C74/B74</f>
+        <v>0.53448949335053819</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75">
+        <v>361228</v>
+      </c>
+      <c r="C75">
+        <v>220292</v>
+      </c>
+      <c r="D75" s="5" t="str">
+        <f>RIGHT(A75,3)</f>
+        <v>png</v>
+      </c>
+      <c r="E75" s="1">
+        <f>C75/B75</f>
         <v>0.60984198345643192</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="8">
-        <f>SUM(B2:B74)</f>
-        <v>56627132</v>
-      </c>
-      <c r="C75" s="8">
-        <f>SUM(C2:C74)</f>
-        <v>14200276</v>
-      </c>
-      <c r="D75" s="4"/>
-      <c r="E75" s="3">
-        <f>C75/B75</f>
-        <v>0.25076805938185248</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A80" s="7" t="s">
+    <row r="76" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="8">
+        <f>SUM(B2:B75)</f>
+        <v>69911803</v>
+      </c>
+      <c r="C76" s="8">
+        <f>SUM(C2:C75)</f>
+        <v>17435904</v>
+      </c>
+      <c r="D76" s="4"/>
+      <c r="E76" s="3">
+        <f>C76/B76</f>
+        <v>0.24939857437234167</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A81" s="7" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E81">
-    <sortCondition ref="D2:D81"/>
-    <sortCondition ref="E2:E81"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E82">
+    <sortCondition ref="D2:D82"/>
+    <sortCondition ref="E2:E82"/>
   </sortState>
   <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="colorScale" priority="1">

</xml_diff>